<commit_message>
Update after leaving Statik and UstUsdc
</commit_message>
<xml_diff>
--- a/PortCrypto02.xlsx
+++ b/PortCrypto02.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C755D085-D337-40C4-B797-1586023FC1BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{738102CB-62B6-4785-872E-735A4B568725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="6" r:id="rId1"/>
@@ -735,27 +735,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.796875" customWidth="1"/>
-    <col min="3" max="3" width="13.796875" customWidth="1"/>
-    <col min="4" max="4" width="14.09765625" customWidth="1"/>
-    <col min="5" max="5" width="13.19921875" customWidth="1"/>
+    <col min="1" max="1" width="10.75" customWidth="1"/>
+    <col min="3" max="3" width="13.75" customWidth="1"/>
+    <col min="4" max="4" width="14.125" customWidth="1"/>
+    <col min="5" max="5" width="13.25" customWidth="1"/>
     <col min="6" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="12.8984375" customWidth="1"/>
-    <col min="10" max="11" width="12.296875" customWidth="1"/>
-    <col min="12" max="12" width="16.19921875" customWidth="1"/>
-    <col min="13" max="13" width="14.8984375" customWidth="1"/>
-    <col min="14" max="14" width="16.59765625" customWidth="1"/>
+    <col min="8" max="8" width="12.875" customWidth="1"/>
+    <col min="10" max="11" width="12.25" customWidth="1"/>
+    <col min="12" max="12" width="16.25" customWidth="1"/>
+    <col min="13" max="13" width="14.875" customWidth="1"/>
+    <col min="14" max="14" width="16.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -797,7 +797,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -817,7 +817,7 @@
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -837,7 +837,7 @@
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -857,7 +857,7 @@
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -877,7 +877,7 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>17</v>
       </c>
@@ -897,7 +897,7 @@
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -917,7 +917,7 @@
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
@@ -937,7 +937,7 @@
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>20</v>
       </c>
@@ -957,7 +957,7 @@
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>21</v>
       </c>
@@ -999,7 +999,7 @@
       </c>
       <c r="N10" s="4"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>22</v>
       </c>
@@ -1083,7 +1083,7 @@
       </c>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>23</v>
       </c>
@@ -1124,7 +1124,7 @@
       </c>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>25</v>
       </c>
@@ -1168,7 +1168,7 @@
       </c>
       <c r="N14" s="4"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
@@ -1210,7 +1210,7 @@
       </c>
       <c r="N15" s="4"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>27</v>
       </c>
@@ -1252,7 +1252,7 @@
       </c>
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>28</v>
       </c>
@@ -1294,7 +1294,7 @@
       </c>
       <c r="N17" s="4"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>29</v>
       </c>
@@ -1336,7 +1336,7 @@
       </c>
       <c r="N18" s="4"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
         <v>30</v>
       </c>
@@ -1378,7 +1378,7 @@
       </c>
       <c r="N19" s="4"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>31</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>44603.959435902776</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>246.44739437442655</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7">
         <v>44603.965493344906</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>246.44739437442655</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>44604.940261377313</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>246.24892578115174</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7">
         <v>44605.629927569447</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>245.98203840425455</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>44606.944312766209</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>246.13130355758489</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7">
         <v>44608.385673032404</v>
       </c>
@@ -1650,8 +1650,8 @@
         <v>247.37795710800407</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
+    <row r="27" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="7">
         <v>44608.662379513888</v>
       </c>
       <c r="B27">
@@ -1686,6 +1686,38 @@
       </c>
       <c r="N27">
         <v>247.37795710800407</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="8">
+        <v>44627.870744143518</v>
+      </c>
+      <c r="B28">
+        <v>530.8596630157848</v>
+      </c>
+      <c r="C28">
+        <v>148.44154814147817</v>
+      </c>
+      <c r="E28">
+        <v>24.106896033595248</v>
+      </c>
+      <c r="F28">
+        <v>0.35999869122139422</v>
+      </c>
+      <c r="G28">
+        <v>97.8460746642603</v>
+      </c>
+      <c r="H28">
+        <v>53.104118372627397</v>
+      </c>
+      <c r="I28">
+        <v>284.57204021004634</v>
+      </c>
+      <c r="L28">
+        <v>20.432078843767346</v>
+      </c>
+      <c r="M28">
+        <v>1.4633222177202497E-4</v>
       </c>
     </row>
   </sheetData>
@@ -1698,29 +1730,29 @@
   <dimension ref="A1:BI30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:A28"/>
+      <selection activeCell="AR29" sqref="AR29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.9" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.8984375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="8.796875" style="10" customWidth="1"/>
+    <col min="1" max="1" width="9.875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="8.75" style="10" customWidth="1"/>
     <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
-    <col min="6" max="9" width="10.09765625" customWidth="1"/>
+    <col min="6" max="9" width="10.125" customWidth="1"/>
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
     <col min="11" max="14" width="0" style="10" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="8.796875" style="10" customWidth="1"/>
+    <col min="16" max="16" width="8.75" style="10" customWidth="1"/>
     <col min="17" max="17" width="0" hidden="1" customWidth="1"/>
     <col min="19" max="21" width="0" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="11.09765625" style="10" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="11.125" style="10" hidden="1" customWidth="1"/>
     <col min="23" max="26" width="0" hidden="1" customWidth="1"/>
     <col min="27" max="38" width="0" style="10" hidden="1" customWidth="1"/>
-    <col min="40" max="40" width="8.796875" style="10" customWidth="1"/>
+    <col min="40" max="40" width="8.75" style="10" customWidth="1"/>
     <col min="42" max="42" width="0" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="8.796875" style="10" customWidth="1"/>
+    <col min="44" max="44" width="8.75" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:61" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="11">
         <f ca="1">OFFSET(A7,0,COUNTA(A7:A27)-1)</f>
         <v>0</v>
@@ -1820,7 +1852,7 @@
       <c r="BH1" s="12"/>
       <c r="BI1" s="12"/>
     </row>
-    <row r="2" spans="1:61" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:61" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
       <c r="C2" s="17" t="s">
         <v>51</v>
@@ -1894,7 +1926,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:61" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:61" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="11"/>
       <c r="B3" s="15"/>
       <c r="C3" s="17" t="s">
@@ -2037,7 +2069,7 @@
         <v>353.95213844318812</v>
       </c>
     </row>
-    <row r="4" spans="1:61" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:61" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>66</v>
       </c>
@@ -2145,7 +2177,7 @@
       <c r="AW4" s="20"/>
       <c r="AX4" s="20"/>
     </row>
-    <row r="5" spans="1:61" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:61" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>67</v>
       </c>
@@ -2258,10 +2290,10 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:61" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:61" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H6" s="10"/>
     </row>
-    <row r="7" spans="1:61" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:61" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>70</v>
       </c>
@@ -2306,7 +2338,7 @@
       <c r="AW7" s="20"/>
       <c r="AX7" s="20"/>
     </row>
-    <row r="8" spans="1:61" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:61" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>72</v>
       </c>
@@ -2340,7 +2372,7 @@
       <c r="AW8" s="20"/>
       <c r="AX8" s="20"/>
     </row>
-    <row r="9" spans="1:61" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:61" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>73</v>
       </c>
@@ -2404,7 +2436,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="10" spans="1:61" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:61" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>75</v>
       </c>
@@ -2463,7 +2495,7 @@
       <c r="AW10" s="20"/>
       <c r="AX10" s="20"/>
     </row>
-    <row r="11" spans="1:61" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:61" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>20</v>
       </c>
@@ -2579,7 +2611,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="12" spans="1:61" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:61" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>22</v>
       </c>
@@ -2606,7 +2638,7 @@
       <c r="AH12" s="15"/>
       <c r="AI12" s="19"/>
     </row>
-    <row r="13" spans="1:61" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:61" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>79</v>
       </c>
@@ -2635,7 +2667,7 @@
       <c r="AH13" s="15"/>
       <c r="AI13" s="19"/>
     </row>
-    <row r="14" spans="1:61" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:61" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="str">
         <f>Foglio1!A13</f>
         <v>23/01/2022</v>
@@ -2701,7 +2733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:61" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:61" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="str">
         <f>Foglio1!A14</f>
         <v>24/01/2022</v>
@@ -2763,7 +2795,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:61" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:61" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="str">
         <f>Foglio1!A15</f>
         <v>31/01/2022</v>
@@ -2815,7 +2847,7 @@
         <v>10.740405681022587</v>
       </c>
     </row>
-    <row r="17" spans="1:44" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:44" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="str">
         <f>Foglio1!A16</f>
         <v>02/02/2022</v>
@@ -2857,7 +2889,7 @@
         <v>11.68009536705989</v>
       </c>
     </row>
-    <row r="18" spans="1:44" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:44" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="str">
         <f>Foglio1!A17</f>
         <v>03/02/2022</v>
@@ -2899,7 +2931,7 @@
         <v>10.022677016147213</v>
       </c>
     </row>
-    <row r="19" spans="1:44" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:44" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="str">
         <f>Foglio1!A18</f>
         <v>04/02/2022</v>
@@ -2941,7 +2973,7 @@
         <v>9.8998196614978884</v>
       </c>
     </row>
-    <row r="20" spans="1:44" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:44" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="str">
         <f>Foglio1!A19</f>
         <v>05/02/2022</v>
@@ -2983,7 +3015,7 @@
         <v>10.694565434798344</v>
       </c>
     </row>
-    <row r="21" spans="1:44" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:44" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="str">
         <f>Foglio1!A20</f>
         <v>11/02/2022</v>
@@ -3025,7 +3057,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:44" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:44" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
         <f>Foglio1!A21</f>
         <v>44603.959435902776</v>
@@ -3067,7 +3099,7 @@
         <v>6.8446686436344564</v>
       </c>
     </row>
-    <row r="23" spans="1:44" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:44" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
         <f>Foglio1!A22</f>
         <v>44603.965493344906</v>
@@ -3109,7 +3141,7 @@
         <v>6.8446686436344564</v>
       </c>
     </row>
-    <row r="24" spans="1:44" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:44" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <f>Foglio1!A23</f>
         <v>44604.940261377313</v>
@@ -3151,7 +3183,7 @@
         <v>4.7695031384103501</v>
       </c>
     </row>
-    <row r="25" spans="1:44" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:44" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <f>Foglio1!A24</f>
         <v>44605.629927569447</v>
@@ -3199,7 +3231,7 @@
         <v>4.790638676709249</v>
       </c>
     </row>
-    <row r="26" spans="1:44" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:44" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <f>Foglio1!A25</f>
         <v>44606.944312766209</v>
@@ -3244,7 +3276,7 @@
         <v>4.5639494192609558</v>
       </c>
     </row>
-    <row r="27" spans="1:44" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:44" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
         <f>Foglio1!A26</f>
         <v>44608.385673032404</v>
@@ -3289,7 +3321,7 @@
         <v>5.3731650266587616</v>
       </c>
     </row>
-    <row r="28" spans="1:44" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:44" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
         <f>Foglio1!A27</f>
         <v>44608.662379513888</v>
@@ -3335,8 +3367,11 @@
         <v>5.3731650266587616</v>
       </c>
     </row>
-    <row r="29" spans="1:44" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
+    <row r="29" spans="1:44" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="11">
+        <f>Foglio1!A28</f>
+        <v>44627.870744143518</v>
+      </c>
       <c r="D29" s="19">
         <f>Foglio1!D28</f>
         <v>0</v>
@@ -3349,11 +3384,11 @@
       <c r="I29" s="21"/>
       <c r="K29" s="19">
         <f>Foglio1!E28</f>
-        <v>0</v>
+        <v>24.106896033595248</v>
       </c>
       <c r="P29" s="19">
         <f>Foglio1!H28</f>
-        <v>0</v>
+        <v>53.104118372627397</v>
       </c>
       <c r="V29" s="19">
         <f>Foglio1!K28</f>
@@ -3370,14 +3405,14 @@
       <c r="AI29" s="19"/>
       <c r="AN29" s="19">
         <f>Foglio1!L28</f>
-        <v>0</v>
+        <v>20.432078843767346</v>
       </c>
       <c r="AR29" s="19">
         <f>Foglio1!M28</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:44" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1.4633222177202497E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:44" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
       <c r="D30" s="19">
         <f>Foglio1!D29</f>

</xml_diff>